<commit_message>
Nearly done posterior distributions section. Haven't done the make-more-interesting updates from this chapter I think.
</commit_message>
<xml_diff>
--- a/Posterior_confidenceIntervalsWar.xlsx
+++ b/Posterior_confidenceIntervalsWar.xlsx
@@ -127,9 +127,6 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -139,18 +136,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="11">
     <dxf>
       <fill>
         <patternFill>
@@ -528,7 +521,7 @@
   <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,14 +543,14 @@
       <c r="A1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
       <c r="K1" t="s">
         <v>9</v>
       </c>
@@ -610,51 +603,51 @@
       <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="D3" s="7">
+      <c r="C3" s="6">
+        <v>0.73</v>
+      </c>
+      <c r="D3" s="6">
         <v>0.5</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>0.5</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="6">
         <v>0.13</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <f>SUMPRODUCT($C3:$F3,$J12:$M12)/SUM($C3:$F3)</f>
-        <v>0.93264248704663211</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4">
+        <v>0.93010752688172049</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3">
         <f>SUM(C3:F3)</f>
-        <v>1.9300000000000002</v>
+        <v>1.8599999999999999</v>
       </c>
       <c r="K3" t="s">
         <v>0</v>
       </c>
-      <c r="L3" s="7">
+      <c r="L3" s="6">
         <f>C3/$I3</f>
-        <v>0.41450777202072536</v>
-      </c>
-      <c r="M3" s="7">
+        <v>0.39247311827956993</v>
+      </c>
+      <c r="M3" s="6">
         <f t="shared" ref="M3:O3" si="0">D3/$I3</f>
-        <v>0.25906735751295334</v>
-      </c>
-      <c r="N3" s="7">
+        <v>0.26881720430107531</v>
+      </c>
+      <c r="N3" s="6">
         <f t="shared" si="0"/>
-        <v>0.25906735751295334</v>
-      </c>
-      <c r="O3" s="7">
+        <v>0.26881720430107531</v>
+      </c>
+      <c r="O3" s="6">
         <f t="shared" si="0"/>
-        <v>6.7357512953367879E-2</v>
-      </c>
-      <c r="P3" s="7">
+        <v>6.9892473118279577E-2</v>
+      </c>
+      <c r="P3" s="6">
         <f>SUMPRODUCT($L3:$O3,$P12:$S12)</f>
-        <v>0.93264248704663211</v>
-      </c>
-      <c r="R3" s="4">
+        <v>0.93010752688172049</v>
+      </c>
+      <c r="R3" s="3">
         <f>SUM(L3:O3)</f>
         <v>1</v>
       </c>
@@ -663,51 +656,51 @@
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>0.09</v>
       </c>
-      <c r="D4" s="7">
-        <v>0.15</v>
-      </c>
-      <c r="E4" s="7">
+      <c r="D4" s="6">
         <v>0.25</v>
       </c>
-      <c r="F4" s="7">
+      <c r="E4" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="F4" s="6">
         <v>0.16</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="6">
         <f t="shared" ref="G4:G6" si="1">SUMPRODUCT($C4:$F4,$J13:$M13)/SUM($C4:$F4)</f>
-        <v>0.86153846153846159</v>
-      </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="3">
         <f t="shared" ref="I4:I6" si="2">SUM(C4:F4)</f>
-        <v>0.65</v>
+        <v>0.75</v>
       </c>
       <c r="K4" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="7">
+      <c r="L4" s="6">
         <f t="shared" ref="L4:L6" si="3">C4/$I4</f>
-        <v>0.13846153846153844</v>
-      </c>
-      <c r="M4" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="M4" s="6">
         <f t="shared" ref="M4:M6" si="4">D4/$I4</f>
-        <v>0.23076923076923075</v>
-      </c>
-      <c r="N4" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="N4" s="6">
         <f t="shared" ref="N4:N6" si="5">E4/$I4</f>
-        <v>0.38461538461538458</v>
-      </c>
-      <c r="O4" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="O4" s="6">
         <f t="shared" ref="O4:O6" si="6">F4/$I4</f>
-        <v>0.24615384615384614</v>
-      </c>
-      <c r="P4" s="7">
+        <v>0.21333333333333335</v>
+      </c>
+      <c r="P4" s="6">
         <f t="shared" ref="P4:P6" si="7">SUMPRODUCT($L4:$O4,$P13:$S13)</f>
-        <v>0.75384615384615383</v>
-      </c>
-      <c r="R4" s="4">
+        <v>0.78666666666666663</v>
+      </c>
+      <c r="R4" s="3">
         <f t="shared" ref="R4:R6" si="8">SUM(L4:O4)</f>
         <v>1</v>
       </c>
@@ -716,51 +709,51 @@
       <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="7">
-        <v>0</v>
-      </c>
-      <c r="D5" s="7">
+      <c r="C5" s="6">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6">
         <v>0.25</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="6">
         <v>0.25</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <v>0.66</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="6">
         <f t="shared" si="1"/>
         <v>0.56896551724137923</v>
       </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="4">
+      <c r="H5" s="2"/>
+      <c r="I5" s="3">
         <f t="shared" si="2"/>
         <v>1.1600000000000001</v>
       </c>
       <c r="K5" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5" s="6">
         <f t="shared" si="4"/>
         <v>0.21551724137931033</v>
       </c>
-      <c r="N5" s="7">
+      <c r="N5" s="6">
         <f t="shared" si="5"/>
         <v>0.21551724137931033</v>
       </c>
-      <c r="O5" s="7">
+      <c r="O5" s="6">
         <f t="shared" si="6"/>
         <v>0.56896551724137923</v>
       </c>
-      <c r="P5" s="7">
+      <c r="P5" s="6">
         <f t="shared" si="7"/>
         <v>0.7844827586206895</v>
       </c>
-      <c r="R5" s="4">
+      <c r="R5" s="3">
         <f t="shared" si="8"/>
         <v>0.99999999999999989</v>
       </c>
@@ -769,51 +762,51 @@
       <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="7">
-        <v>0.11</v>
-      </c>
-      <c r="D6" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="E6" s="7">
-        <v>0</v>
-      </c>
-      <c r="F6" s="7">
+      <c r="C6" s="6">
+        <v>0.18</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6">
         <v>0.05</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="6">
         <f t="shared" si="1"/>
-        <v>0.38461538461538464</v>
-      </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3">
         <f t="shared" si="2"/>
-        <v>0.26</v>
+        <v>0.22999999999999998</v>
       </c>
       <c r="K6" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6" s="6">
         <f t="shared" si="3"/>
-        <v>0.42307692307692307</v>
-      </c>
-      <c r="M6" s="7">
+        <v>0.78260869565217395</v>
+      </c>
+      <c r="M6" s="6">
         <f t="shared" si="4"/>
-        <v>0.38461538461538464</v>
-      </c>
-      <c r="N6" s="7">
+        <v>0</v>
+      </c>
+      <c r="N6" s="6">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O6" s="7">
+      <c r="O6" s="6">
         <f t="shared" si="6"/>
-        <v>0.19230769230769232</v>
-      </c>
-      <c r="P6" s="7">
+        <v>0.21739130434782611</v>
+      </c>
+      <c r="P6" s="6">
         <f t="shared" si="7"/>
-        <v>0.80769230769230771</v>
-      </c>
-      <c r="R6" s="4">
+        <v>0.78260869565217395</v>
+      </c>
+      <c r="R6" s="3">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
@@ -822,80 +815,80 @@
       <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <f>SUM(C3:C6)</f>
         <v>1</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <f t="shared" ref="D7:F7" si="9">SUM(D3:D6)</f>
         <v>1</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <f>SUMPRODUCT(C$3:C$6,J$12:J$15)</f>
-        <v>0.8</v>
-      </c>
-      <c r="D8" s="7">
+        <v>0.82</v>
+      </c>
+      <c r="D8" s="6">
         <f>SUMPRODUCT(D$3:D$6,K$12:K$15)</f>
         <v>0.75</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <f>SUMPRODUCT(E$3:E$6,L$12:L$15)</f>
         <v>0.75</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <f>SUMPRODUCT(F$3:F$6,M$12:M$15)</f>
         <v>0.82000000000000006</v>
       </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
       <c r="I10" t="s">
         <v>4</v>
       </c>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
       <c r="O10" t="s">
         <v>7</v>
       </c>
-      <c r="P10" s="5" t="s">
+      <c r="P10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
@@ -931,7 +924,7 @@
       <c r="M11" t="s">
         <v>16</v>
       </c>
-      <c r="N11" s="5"/>
+      <c r="N11" s="4"/>
       <c r="O11" s="1" t="s">
         <v>11</v>
       </c>
@@ -952,54 +945,54 @@
       <c r="B12" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <f>C3</f>
-        <v>0.8</v>
-      </c>
-      <c r="D12" s="7">
+        <v>0.73</v>
+      </c>
+      <c r="D12" s="6">
         <f t="shared" ref="D12:F12" si="10">D3</f>
         <v>0.5</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <f t="shared" si="10"/>
         <v>0.5</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <f t="shared" si="10"/>
         <v>0.13</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="6">
         <f>SUMPRODUCT($C12:$F12,$P12:$S12)/SUM($C12:$F12)</f>
-        <v>0.93264248704663211</v>
+        <v>0.93010752688172049</v>
       </c>
       <c r="I12" t="s">
         <v>0</v>
       </c>
-      <c r="J12" s="6">
-        <v>1</v>
-      </c>
-      <c r="K12" s="6">
-        <v>1</v>
-      </c>
-      <c r="L12" s="6">
-        <v>1</v>
-      </c>
-      <c r="M12" s="6">
+      <c r="J12" s="5">
+        <v>1</v>
+      </c>
+      <c r="K12" s="5">
+        <v>1</v>
+      </c>
+      <c r="L12" s="5">
+        <v>1</v>
+      </c>
+      <c r="M12" s="5">
         <v>0</v>
       </c>
       <c r="O12" t="s">
         <v>0</v>
       </c>
-      <c r="P12" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="6">
-        <v>1</v>
-      </c>
-      <c r="R12" s="6">
-        <v>1</v>
-      </c>
-      <c r="S12" s="6">
+      <c r="P12" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="5">
+        <v>1</v>
+      </c>
+      <c r="R12" s="5">
+        <v>1</v>
+      </c>
+      <c r="S12" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1007,55 +1000,55 @@
       <c r="B13" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <f t="shared" ref="C13:F13" si="11">C4</f>
         <v>0.09</v>
       </c>
-      <c r="D13" s="7">
-        <f t="shared" si="11"/>
-        <v>0.15</v>
-      </c>
-      <c r="E13" s="7">
+      <c r="D13" s="6">
         <f t="shared" si="11"/>
         <v>0.25</v>
       </c>
-      <c r="F13" s="7">
+      <c r="E13" s="6">
+        <f t="shared" si="11"/>
+        <v>0.25</v>
+      </c>
+      <c r="F13" s="6">
         <f t="shared" si="11"/>
         <v>0.16</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="6">
         <f>SUMPRODUCT($C13:$F13,$P13:$S13)/SUM($C13:$F13)</f>
-        <v>0.75384615384615383</v>
+        <v>0.78666666666666663</v>
       </c>
       <c r="I13" t="s">
         <v>1</v>
       </c>
-      <c r="J13" s="6">
-        <v>0</v>
-      </c>
-      <c r="K13" s="6">
-        <v>1</v>
-      </c>
-      <c r="L13" s="6">
-        <v>1</v>
-      </c>
-      <c r="M13" s="6">
-        <v>1</v>
-      </c>
-      <c r="N13" s="4"/>
+      <c r="J13" s="5">
+        <v>1</v>
+      </c>
+      <c r="K13" s="5">
+        <v>1</v>
+      </c>
+      <c r="L13" s="5">
+        <v>1</v>
+      </c>
+      <c r="M13" s="5">
+        <v>1</v>
+      </c>
+      <c r="N13" s="3"/>
       <c r="O13" t="s">
         <v>1</v>
       </c>
-      <c r="P13" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="6">
-        <v>1</v>
-      </c>
-      <c r="R13" s="6">
-        <v>1</v>
-      </c>
-      <c r="S13" s="6">
+      <c r="P13" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="5">
+        <v>1</v>
+      </c>
+      <c r="R13" s="5">
+        <v>1</v>
+      </c>
+      <c r="S13" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1063,55 +1056,55 @@
       <c r="B14" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <f t="shared" ref="C14:F14" si="12">C5</f>
         <v>0</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="6">
         <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="6">
         <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="6">
         <f t="shared" si="12"/>
         <v>0.66</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="6">
         <f>SUMPRODUCT($C14:$F14,$P14:$S14)/SUM($C14:$F14)</f>
         <v>0.78448275862068961</v>
       </c>
       <c r="I14" t="s">
         <v>2</v>
       </c>
-      <c r="J14" s="6">
-        <v>0</v>
-      </c>
-      <c r="K14" s="6">
-        <v>0</v>
-      </c>
-      <c r="L14" s="6">
-        <v>0</v>
-      </c>
-      <c r="M14" s="6">
-        <v>1</v>
-      </c>
-      <c r="N14" s="3"/>
+      <c r="J14" s="5">
+        <v>0</v>
+      </c>
+      <c r="K14" s="5">
+        <v>0</v>
+      </c>
+      <c r="L14" s="5">
+        <v>0</v>
+      </c>
+      <c r="M14" s="5">
+        <v>1</v>
+      </c>
+      <c r="N14" s="2"/>
       <c r="O14" t="s">
         <v>2</v>
       </c>
-      <c r="P14" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="6">
-        <v>0</v>
-      </c>
-      <c r="R14" s="6">
-        <v>1</v>
-      </c>
-      <c r="S14" s="6">
+      <c r="P14" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="5">
+        <v>0</v>
+      </c>
+      <c r="R14" s="5">
+        <v>1</v>
+      </c>
+      <c r="S14" s="5">
         <v>1</v>
       </c>
     </row>
@@ -1119,55 +1112,55 @@
       <c r="B15" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <f t="shared" ref="C15:F15" si="13">C6</f>
-        <v>0.11</v>
-      </c>
-      <c r="D15" s="7">
+        <v>0.18</v>
+      </c>
+      <c r="D15" s="6">
         <f t="shared" si="13"/>
-        <v>0.1</v>
-      </c>
-      <c r="E15" s="7">
+        <v>0</v>
+      </c>
+      <c r="E15" s="6">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="6">
         <f t="shared" si="13"/>
         <v>0.05</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="6">
         <f>SUMPRODUCT($C15:$F15,$P15:$S15)/SUM($C15:$F15)</f>
-        <v>0.80769230769230771</v>
+        <v>0.78260869565217395</v>
       </c>
       <c r="I15" t="s">
         <v>12</v>
       </c>
-      <c r="J15" s="6">
-        <v>0</v>
-      </c>
-      <c r="K15" s="6">
-        <v>1</v>
-      </c>
-      <c r="L15" s="6">
-        <v>0</v>
-      </c>
-      <c r="M15" s="6">
-        <v>0</v>
-      </c>
-      <c r="N15" s="3"/>
+      <c r="J15" s="5">
+        <v>0</v>
+      </c>
+      <c r="K15" s="5">
+        <v>0</v>
+      </c>
+      <c r="L15" s="5">
+        <v>0</v>
+      </c>
+      <c r="M15" s="5">
+        <v>0</v>
+      </c>
+      <c r="N15" s="2"/>
       <c r="O15" t="s">
         <v>12</v>
       </c>
-      <c r="P15" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="6">
-        <v>1</v>
-      </c>
-      <c r="R15" s="6">
-        <v>0</v>
-      </c>
-      <c r="S15" s="6">
+      <c r="P15" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="5">
+        <v>0</v>
+      </c>
+      <c r="R15" s="5">
+        <v>0</v>
+      </c>
+      <c r="S15" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1175,52 +1168,52 @@
       <c r="B16" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <f>SUMPRODUCT(C$12:C$15,P$12:P$15)/SUM(C$12:C$15)</f>
         <v>1</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="6">
         <f>SUMPRODUCT(D$12:D$15,Q$12:Q$15)/SUM(D$12:D$15)</f>
         <v>0.75</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="6">
         <f>SUMPRODUCT(E$12:E$15,R$12:R$15)/SUM(E$12:E$15)</f>
         <v>1</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="6">
         <f>SUMPRODUCT(F$12:F$15,S$12:S$15)/SUM(F$12:F$15)</f>
         <v>0.66</v>
       </c>
-      <c r="G16" s="7"/>
-      <c r="K16" s="6"/>
-      <c r="N16" s="4"/>
+      <c r="G16" s="6"/>
+      <c r="K16" s="5"/>
+      <c r="N16" s="3"/>
     </row>
     <row r="17" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="G17" s="7"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
+      <c r="G17" s="6"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C18" s="7">
-        <v>1</v>
-      </c>
-      <c r="D18" s="7">
-        <v>1</v>
-      </c>
-      <c r="E18" s="7">
-        <v>1</v>
-      </c>
-      <c r="F18" s="7">
-        <v>1</v>
-      </c>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
+      <c r="C18" s="6">
+        <v>1</v>
+      </c>
+      <c r="D18" s="6">
+        <v>1</v>
+      </c>
+      <c r="E18" s="6">
+        <v>1</v>
+      </c>
+      <c r="F18" s="6">
+        <v>1</v>
+      </c>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1228,57 +1221,57 @@
     <mergeCell ref="C10:F10"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:F6">
-    <cfRule type="expression" dxfId="11" priority="11">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>$J$12:$M$15=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:F6">
-    <cfRule type="expression" dxfId="10" priority="10">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>J12=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:F15">
-    <cfRule type="expression" dxfId="9" priority="9">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>P12=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13:F15">
-    <cfRule type="expression" dxfId="8" priority="8">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>P13=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:F8">
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>C8&lt;0.75</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:G15">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>G12&lt;0.75</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:F7">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>C7&lt;&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:F16">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>C16&lt;0.75</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G6">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>G3&lt;0.75</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:O3">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>P12=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:O6">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>P13=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>